<commit_message>
nullable parameters of unitcleaners updated
</commit_message>
<xml_diff>
--- a/openergy/configurators/resources/multiclean_config_model.xlsx
+++ b/openergy/configurators/resources/multiclean_config_model.xlsx
@@ -190,8 +190,173 @@
     <t>Write an optional comment for the series.</t>
   </si>
   <si>
-    <t>By default, this field is set equal to the Input Time Extensivity.
-If you want to modify the output type, choose between the 4 following categories:
+    <t>Openration Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have to perform python code in this cell using 4 spaces as incrementation.
+If you want to perform a transformation on the Output Series.
+Example: a 4-20 mA sensor measure a temperature between -20 and 150°C.
+The input series corresponds to the 4-20 mA signal you want to convert to °C. 
+Enter the following Operation Function:
+def fct(value):   
+    value =  (value-4)*(150-(-20))/(20-4)+(-20)
+    return value
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have to perform python code in this cell using 4 spaces as incrementation.
+If you want to perform a filter on the output Series.
+The filtered values will be replaced by NaNs.
+Example: you want to filter values of an indoor temperature that are below 10°C and above 50°C:
+def fct(value):    #Apply a filter on your values. Return true to keep values, else false.
+    condition = (value &lt;10 or value &gt;50)
+    return condition
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have to perform python code in this cell using 4 spaces as incrementation.
+If you want to perform a filter on the time derivateive of the output Series.
+The filtered values will be replaced by NaNs.
+Example: you want to filter values of an indoor temperature that change faster than 1°C/minute:
+def fct(value):   
+    condition = (abs(value) &gt; 1./60) # time derivative of a temperature is given in °C/s
+    return condition
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For experts only, see documentation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This totally free function is applied before the whole cleaning workflow.
+(If the proposed wrokflow doesn't match your needs).
+For experts only.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of time steps necessary before a value so that it can be calculated.
+Only if a Custom Function is defined.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of time steps necessary after a value so that it can be calculated.
+Only if a Custom Function is defined.
+</t>
+  </si>
+  <si>
+    <t>This field has to be checked with a 'X' so that the config of the row is taken into account while uploading the file. It enables you to configure only the series of your choice. If you don't want to modify or config a series, leave this field blank.</t>
+  </si>
+  <si>
+    <t>Series:</t>
+  </si>
+  <si>
+    <t>Configured Series:</t>
+  </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>True : the cleaning will be running once you saved the config
+False : the cleaning config will be saved but the series won't be cleaned 
+Note that is still possible to modify the running status directly on the tab "Monitor" of the platform, but only series by series.</t>
+  </si>
+  <si>
+    <t>Input is Regular</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The delay from which data are considered to be late for Analyses scripts.
+Late data will be temporarily filled by NaNs until real data arrive (Analyses can then keep on running).
+This value must be written as a Pandas frequency 
+Example: 6H,D,2D,W,... By default this value is set at 6 hours.
+Example: Weather webservice SYNOP is supposed to send weather data every hour.
+However, it often happens that no data is sent for 2 hours, and that the missing data are sent together with the third hour.
+In that case, you may want to enter a Wait offset = 3H, to make sure that this type of delay is taken into account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">By default (if left empty), this filed is set to '6H'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The maximum number of consecutive empty time steps you consider reasonable to fill by linear interpolation.
+In case of longer blanks, they will be filled bay NaNs.
+Example: for a hourly temperature, you may want to fill blanks no longer than 3 hours; in that case, set Interpolate Limit to 3.
+Note that if Interpolate Limit = 0, no interpolation is performed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t>By default (if left empty), this field is set to 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This field describes how to resample an instantaneous output series. 2 choices are available:
+- Mean: well suited for temperatures, pressure, etc.
+- First: well suited for energy index, volume index, etc.
+Note the Output Resample Rule is automatically selected if Output Time Extensivity = Delta, Mean or Mean Derivative.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t>By default (if left empty), this field is set to 'Mean'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you want to modify the output type, choose between the 4 following categories:
 - Instantaneous: a time intensive quantity measured at the recorded time stamp.
 This category is well suited for: (instantaneous) temperature, humidity, pressure, power, flow, energy index...
 Example: Meteo France records the instantaneous drybulb temperature each hour.
@@ -202,105 +367,19 @@
 This category is well suited for: (averaged) temperature, humidity, pressure, power, flow,...
 Example: mean temperature of a room between 12:00 and 13:00. 
 - Mean Derivative: the time derivative of the input series, averaged over the time step.
-This category is well suited to get the power out of energy delta, flow out of volume, etc...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This field describes how to resample an instantaneous output series. 2 choices are available:
-- Mean: well suited for temperatures, pressure, etc.
-- First: well suited for energy index, volume index, etc.
-Note the Output Resample Rule is automatically selected if Output Time Extensivity = Delta, Mean or Mean Derivative.
+This category is well suited to get the power out of energy delta, flow out of volume, etc...
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive empty time steps you consider reasonable to fill by linear interpolation.
-In case of longer blanks, they will be filled bay NaNs.
-Example: for a hourly temperature, you may want to fill blanks no longer than 3 hours; in that case, set Interpolate Limit to 3.
-Note that if Interpolate Limit = 0, no interpolation is performed.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The delay from which data are considered to be late for Analyses scripts.
-Late data will be temporarily filled by NaNs until real data arrive (Analyses can then keep on running).
-This value must be written as a Pandas frequency 
-Example: 6H,D,2D,W,... By default this value is set at 6 hours.
-Example: Weather webservice SYNOP is supposed to send weather data every hour.
-However, it often happens that no data is sent for 2 hours, and that the missing data are sent together with the third hour.
-In that case, you may want to enter a Wait offset = 3H, to make sure that this type of delay is taken into account.
-</t>
-  </si>
-  <si>
-    <t>Openration Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have to perform python code in this cell using 4 spaces as incrementation.
-If you want to perform a transformation on the Output Series.
-Example: a 4-20 mA sensor measure a temperature between -20 and 150°C.
-The input series corresponds to the 4-20 mA signal you want to convert to °C. 
-Enter the following Operation Function:
-def fct(value):   
-    value =  (value-4)*(150-(-20))/(20-4)+(-20)
-    return value
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have to perform python code in this cell using 4 spaces as incrementation.
-If you want to perform a filter on the output Series.
-The filtered values will be replaced by NaNs.
-Example: you want to filter values of an indoor temperature that are below 10°C and above 50°C:
-def fct(value):    #Apply a filter on your values. Return true to keep values, else false.
-    condition = (value &lt;10 or value &gt;50)
-    return condition
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have to perform python code in this cell using 4 spaces as incrementation.
-If you want to perform a filter on the time derivateive of the output Series.
-The filtered values will be replaced by NaNs.
-Example: you want to filter values of an indoor temperature that change faster than 1°C/minute:
-def fct(value):   
-    condition = (abs(value) &gt; 1./60) # time derivative of a temperature is given in °C/s
-    return condition
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For experts only, see documentation
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This totally free function is applied before the whole cleaning workflow.
-(If the proposed wrokflow doesn't match your needs).
-For experts only.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of time steps necessary before a value so that it can be calculated.
-Only if a Custom Function is defined.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of time steps necessary after a value so that it can be calculated.
-Only if a Custom Function is defined.
-</t>
-  </si>
-  <si>
-    <t>This field has to be checked with a 'X' so that the config of the row is taken into account while uploading the file. It enables you to configure only the series of your choice. If you don't want to modify or config a series, leave this field blank.</t>
-  </si>
-  <si>
-    <t>Series:</t>
-  </si>
-  <si>
-    <t>Configured Series:</t>
-  </si>
-  <si>
-    <t>Running</t>
-  </si>
-  <si>
-    <t>True : the cleaning will be running once you saved the config
-False : the cleaning config will be saved but the series won't be cleaned 
-Note that is still possible to modify the running status directly on the tab "Monitor" of the platform, but only series by series.</t>
-  </si>
-  <si>
-    <t>Input is Regular</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t>By default (if left empty), this field is set equal to the Input Time Extensivity.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -930,6 +1009,9 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -995,9 +1077,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1352,7 +1431,7 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1428,7 +1507,7 @@
     </row>
     <row r="4" spans="1:23" s="14" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" s="13">
         <f>COUNTA(A:A) - 6</f>
@@ -1453,7 +1532,7 @@
     </row>
     <row r="5" spans="1:23" s="14" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="49">
         <f>COUNTA(C:C) - 1</f>
@@ -1483,31 +1562,31 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="58"/>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="70" t="s">
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="64" t="s">
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="67"/>
     </row>
     <row r="7" spans="1:23" s="14" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1520,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>10</v>
@@ -1544,7 +1623,7 @@
         <v>16</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>17</v>
@@ -1581,8 +1660,8 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1602,7 +1681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A37" sqref="A37:L37"/>
     </sheetView>
   </sheetViews>
@@ -1615,10 +1694,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="78"/>
       <c r="C1" s="16" t="s">
         <v>28</v>
       </c>
@@ -1635,10 +1714,10 @@
       <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="20" t="s">
         <v>29</v>
       </c>
@@ -1659,20 +1738,20 @@
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="83"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="84"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
@@ -1693,20 +1772,20 @@
       <c r="L6" s="46"/>
     </row>
     <row r="7" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="81"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="52" t="s">
@@ -1725,24 +1804,24 @@
       <c r="L9" s="54"/>
     </row>
     <row r="10" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="80"/>
+      <c r="A10" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="81"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -1757,20 +1836,20 @@
       <c r="L12" s="62"/>
     </row>
     <row r="13" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="78" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="80"/>
+      <c r="A13" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="81"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
@@ -1791,20 +1870,20 @@
       <c r="L15" s="48"/>
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="81"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
@@ -1825,20 +1904,20 @@
       <c r="L18" s="46"/>
     </row>
     <row r="19" spans="1:13" ht="206" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="80"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="25"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1876,20 +1955,20 @@
       <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="80"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="81"/>
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1915,20 +1994,20 @@
       <c r="L24" s="46"/>
     </row>
     <row r="25" spans="1:13" ht="145" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="80"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="81"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="43" t="s">
@@ -1949,20 +2028,20 @@
       <c r="L27" s="46"/>
     </row>
     <row r="28" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="80"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="81"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="43" t="s">
@@ -1983,20 +2062,20 @@
       <c r="L30" s="46"/>
     </row>
     <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="79"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="80"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="81"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="25"/>
@@ -2031,38 +2110,38 @@
       <c r="L33" s="46"/>
     </row>
     <row r="34" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="80"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="81"/>
     </row>
     <row r="35" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
     </row>
     <row r="36" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="32" t="s">
@@ -2110,21 +2189,21 @@
       <c r="K39" s="27"/>
       <c r="L39" s="28"/>
     </row>
-    <row r="40" spans="1:12" ht="273" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="78" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="79"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="79"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="79"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="79"/>
-      <c r="L40" s="80"/>
+    <row r="40" spans="1:12" ht="291" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="80"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="80"/>
+      <c r="L40" s="81"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
@@ -2144,21 +2223,21 @@
       <c r="K42" s="27"/>
       <c r="L42" s="28"/>
     </row>
-    <row r="43" spans="1:12" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="73" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="74"/>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="75"/>
+    <row r="43" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="75"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="76"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
@@ -2178,21 +2257,21 @@
       <c r="K45" s="27"/>
       <c r="L45" s="28"/>
     </row>
-    <row r="46" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="74"/>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="75"/>
+    <row r="46" spans="1:12" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="75"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
+      <c r="I46" s="75"/>
+      <c r="J46" s="75"/>
+      <c r="K46" s="75"/>
+      <c r="L46" s="76"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="26" t="s">
@@ -2212,25 +2291,25 @@
       <c r="K48" s="27"/>
       <c r="L48" s="28"/>
     </row>
-    <row r="49" spans="1:12" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="74"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="74"/>
-      <c r="K49" s="74"/>
-      <c r="L49" s="75"/>
+    <row r="49" spans="1:12" ht="148" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="75"/>
+      <c r="K49" s="75"/>
+      <c r="L49" s="76"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B51" s="27"/>
       <c r="C51" s="32" t="s">
@@ -2247,20 +2326,20 @@
       <c r="L51" s="28"/>
     </row>
     <row r="52" spans="1:12" ht="181" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="74"/>
-      <c r="C52" s="74"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="74"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="75"/>
+      <c r="A52" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="75"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
+      <c r="L52" s="76"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
@@ -2281,20 +2360,20 @@
       <c r="L54" s="28"/>
     </row>
     <row r="55" spans="1:12" ht="148" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="74"/>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
-      <c r="G55" s="74"/>
-      <c r="H55" s="74"/>
-      <c r="I55" s="74"/>
-      <c r="J55" s="74"/>
-      <c r="K55" s="74"/>
-      <c r="L55" s="75"/>
+      <c r="A55" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="75"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
+      <c r="I55" s="75"/>
+      <c r="J55" s="75"/>
+      <c r="K55" s="75"/>
+      <c r="L55" s="76"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="25"/>
@@ -2329,20 +2408,20 @@
       <c r="L57" s="28"/>
     </row>
     <row r="58" spans="1:12" ht="145" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="74"/>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
-      <c r="I58" s="74"/>
-      <c r="J58" s="74"/>
-      <c r="K58" s="74"/>
-      <c r="L58" s="75"/>
+      <c r="A58" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="75"/>
+      <c r="C58" s="75"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="75"/>
+      <c r="F58" s="75"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="75"/>
+      <c r="I58" s="75"/>
+      <c r="J58" s="75"/>
+      <c r="K58" s="75"/>
+      <c r="L58" s="76"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
@@ -2363,20 +2442,20 @@
       <c r="L60" s="31"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="B61" s="74"/>
-      <c r="C61" s="74"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="74"/>
-      <c r="H61" s="74"/>
-      <c r="I61" s="74"/>
-      <c r="J61" s="74"/>
-      <c r="K61" s="74"/>
-      <c r="L61" s="75"/>
+      <c r="A61" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="75"/>
+      <c r="C61" s="75"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
+      <c r="F61" s="75"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="75"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="75"/>
+      <c r="K61" s="75"/>
+      <c r="L61" s="76"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="29" t="s">
@@ -2397,20 +2476,20 @@
       <c r="L63" s="31"/>
     </row>
     <row r="64" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="78" t="s">
-        <v>55</v>
-      </c>
-      <c r="B64" s="79"/>
-      <c r="C64" s="79"/>
-      <c r="D64" s="79"/>
-      <c r="E64" s="79"/>
-      <c r="F64" s="79"/>
-      <c r="G64" s="79"/>
-      <c r="H64" s="79"/>
-      <c r="I64" s="79"/>
-      <c r="J64" s="79"/>
-      <c r="K64" s="79"/>
-      <c r="L64" s="80"/>
+      <c r="A64" s="79" t="s">
+        <v>51</v>
+      </c>
+      <c r="B64" s="80"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="80"/>
+      <c r="E64" s="80"/>
+      <c r="F64" s="80"/>
+      <c r="G64" s="80"/>
+      <c r="H64" s="80"/>
+      <c r="I64" s="80"/>
+      <c r="J64" s="80"/>
+      <c r="K64" s="80"/>
+      <c r="L64" s="81"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="29" t="s">
@@ -2431,20 +2510,20 @@
       <c r="L66" s="31"/>
     </row>
     <row r="67" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="B67" s="74"/>
-      <c r="C67" s="74"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="74"/>
-      <c r="I67" s="74"/>
-      <c r="J67" s="74"/>
-      <c r="K67" s="74"/>
-      <c r="L67" s="75"/>
+      <c r="A67" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="75"/>
+      <c r="C67" s="75"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
+      <c r="G67" s="75"/>
+      <c r="H67" s="75"/>
+      <c r="I67" s="75"/>
+      <c r="J67" s="75"/>
+      <c r="K67" s="75"/>
+      <c r="L67" s="76"/>
     </row>
     <row r="68" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -2466,20 +2545,20 @@
       <c r="L69" s="31"/>
     </row>
     <row r="70" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="73" t="s">
-        <v>57</v>
-      </c>
-      <c r="B70" s="74"/>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="74"/>
-      <c r="K70" s="74"/>
-      <c r="L70" s="75"/>
+      <c r="A70" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="75"/>
+      <c r="C70" s="75"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="75"/>
+      <c r="F70" s="75"/>
+      <c r="G70" s="75"/>
+      <c r="H70" s="75"/>
+      <c r="I70" s="75"/>
+      <c r="J70" s="75"/>
+      <c r="K70" s="75"/>
+      <c r="L70" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>